<commit_message>
changed name mail to Email on DB.xlsx
</commit_message>
<xml_diff>
--- a/userservice/src/main/resources/DB.xlsx
+++ b/userservice/src/main/resources/DB.xlsx
@@ -28,9 +28,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>mail</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -41,6 +38,9 @@
   </si>
   <si>
     <t>surname</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,22 +410,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>